<commit_message>
removed pdfs and reformatted readme and data dict
</commit_message>
<xml_diff>
--- a/resources/seqr_metadata_templates/Template_data_dictionaries/individuals_metadata_template data dictionary.xlsx
+++ b/resources/seqr_metadata_templates/Template_data_dictionaries/individuals_metadata_template data dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwfor/Code/rare-disease/resources/seqr_metadata_templates/Template_data_dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B1A1BF-95BE-4343-91D3-F02FB4D68FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B28F4D-4E88-F54E-9B02-E61D25473389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>Expected Mode of Inheritance</t>
   </si>
   <si>
-    <t>comma-separated list of the following: Sporadic, Autosomal dominant inheritance, Sex-limited autosomal dominant, Male-limited autosomal dominant, Autosomal dominant contiguous gene syndrome, Autosomal recessive inheritance, Gonosomal inheritance, X-linked inheritance, X-linked recessive inheritance, Y-linked inheritance, X-linked dominant inheritance, Multifactorial inheritance, Mitochondrial inheritance</t>
-  </si>
-  <si>
     <t>Fertility Medications</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>One of the following: Congenital onset, Embryonal onset, Fetal onset, Neonatal onset, Infantile onset, Childhood onset, Juvenile onset,  Young adult onset, Adult onset, Middle age onset, Late onset</t>
+  </si>
+  <si>
+    <t>Comma-separated list of the following: Sporadic, Autosomal dominant inheritance, Sex-limited autosomal dominant, Male-limited autosomal dominant, Autosomal dominant contiguous gene syndrome, Autosomal recessive inheritance, Gonosomal inheritance, X-linked inheritance, X-linked recessive inheritance, Y-linked inheritance, X-linked dominant inheritance, Multifactorial inheritance, Mitochondrial inheritance</t>
   </si>
 </sst>
 </file>
@@ -285,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -301,8 +301,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,14 +619,14 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>46</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -655,13 +661,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>23</v>
@@ -670,7 +676,7 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>23</v>
@@ -679,7 +685,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>23</v>
@@ -688,7 +694,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>23</v>
@@ -697,7 +703,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>23</v>
@@ -706,7 +712,7 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>23</v>
@@ -715,7 +721,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>23</v>
@@ -724,72 +730,72 @@
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="11"/>
       <c r="B28" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="12"/>
       <c r="B29" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>